<commit_message>
rebuild cache to background tasks
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleksandr/Desktop/YLab/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929BCEBA-34DB-964F-A6E8-D3F2EF200315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03A89BD-E57F-F442-B779-4CF1E16ADC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4800" windowWidth="27040" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,7 +489,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -774,7 +774,7 @@
         <v>34</v>
       </c>
       <c r="F18" s="1">
-        <v>888.08</v>
+        <v>1111.08</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>